<commit_message>
Think I'm done for the night. Starting to get tired. Will finish this off tomorrow, probably.
</commit_message>
<xml_diff>
--- a/A2/Workspace.excel.xlsx
+++ b/A2/Workspace.excel.xlsx
@@ -8,35 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tyler\School\2025 Winter\Introduction to Cryptography\4520Labs\A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B63EF68-8861-4164-B81F-9CADA690A865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCA5A9D-3CE4-4E1D-9EA3-49EF8714F272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>A</t>
   </si>
@@ -102,6 +92,111 @@
   </si>
   <si>
     <t>THESERGEANTATARMS</t>
+  </si>
+  <si>
+    <t>0809030206071A171A081C07141D</t>
+  </si>
+  <si>
+    <t>00051311191119070D091B08130B</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>In binary:</t>
+  </si>
+  <si>
+    <t>GORGEOUS SUSAN</t>
+  </si>
+  <si>
+    <t>NICOTINE IS BAD</t>
+  </si>
+  <si>
+    <t>MARIJUANAS LEGAL</t>
+  </si>
+  <si>
+    <t>JUSTINE TRUDEAU</t>
+  </si>
+  <si>
+    <t>FLOYD MAYWEATHER</t>
+  </si>
+  <si>
+    <t>ANGELINA JOLIE</t>
+  </si>
+  <si>
+    <t>EMBEZZLED FUNDS</t>
+  </si>
+  <si>
+    <t>NANETTE WORKMAN</t>
+  </si>
+  <si>
+    <t>ELIZABETH MAY</t>
+  </si>
+  <si>
+    <t>Cryptext 1</t>
+  </si>
+  <si>
+    <t>Cryptext 2</t>
+  </si>
+  <si>
+    <t>GRANT US PEACE</t>
+  </si>
+  <si>
+    <t>WE'RE AWESOME</t>
+  </si>
+  <si>
+    <t>Potential Messages</t>
+  </si>
+  <si>
+    <t>0000100000001001000000110000001000000110000001110001101000010111000110100000100000011100000001110001010000011101</t>
+  </si>
+  <si>
+    <t>0000000000000101000100110001000100011001000100010001100100000111000011010000100100011011000010000001001100001011</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>01001111 01000110 01010001 01000101 01000011 01001000 01001111 01000100 00111010 01011011 01001001 01010100 01010101 01010011 00000010</t>
+  </si>
+  <si>
+    <t>01001101 01000101 01001010 01011000 01000111 01000101 01011111 01000011 01010010 00101000 01010001 01000110 01001101 00010111 00000010</t>
+  </si>
+  <si>
+    <t>01000110 01000000 01000000 01001101 01010010 01001110 01010100 01010010 00111010 01000001 01001111 00100111 01010110 01011100 01001100 00000011 00001001</t>
+  </si>
+  <si>
+    <t>01000101 01001000 01010001 01001011 01001100 01010010 01011011 01011001 01011011 01011011 00111100 01001011 01010001 01011010 01001001 01000101 00001001 00001000</t>
+  </si>
+  <si>
+    <t>01000010 01011100 01010000 01010110 01001111 01001001 01011111 00110111 01001110 01011010 01001001 01000011 01010001 01011100 01011101</t>
+  </si>
+  <si>
+    <t>01001110 01000101 01001100 01011011 01000010 00100111 01010111 01010110 01000011 01011111 01011001 01000110 01000000 01010101 01001101 01011011</t>
+  </si>
+  <si>
+    <t>01001001 01000111 01000100 01000111 01001010 01001110 01010100 01010110 00111010 01000010 01010011 01001011 01011101 01011000</t>
+  </si>
+  <si>
+    <t>01001101 01000100 01000001 01000111 01011100 01011101 01010110 01010010 01011110 00101000 01011010 01010010 01011010 01011001 01011011</t>
+  </si>
+  <si>
+    <t>01000110 01001000 01001101 01000111 01010010 01010011 01011111 00110111 01001101 01000111 01001110 01001100 01011001 01011100 01000110</t>
+  </si>
+  <si>
+    <t>01001111 01011011 01000010 01001100 01010010 00100111 01001111 01000100 00111010 01011000 01011001 01000110 01010111 01011000</t>
+  </si>
+  <si>
+    <t>01011111 01001100 00100100 01010000 01000011 00100111 01011011 01000000 01011111 01011011 01010011 01001010 01010001</t>
+  </si>
+  <si>
+    <t>Corresponding Key for M1</t>
+  </si>
+  <si>
+    <t>Decrypted M2:</t>
+  </si>
+  <si>
+    <t>Found it!</t>
   </si>
 </sst>
 </file>
@@ -142,11 +237,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:BP32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AT20" sqref="AT20:BJ32"/>
     </sheetView>
   </sheetViews>
@@ -1187,7 +1283,7 @@
         <v>-12</v>
       </c>
       <c r="AX13">
-        <f t="shared" ref="AU13:BI13" si="19">AX9-AX11</f>
+        <f t="shared" ref="AX13:BI13" si="19">AX9-AX11</f>
         <v>14</v>
       </c>
       <c r="AY13">
@@ -1901,7 +1997,7 @@
         <v>-18</v>
       </c>
       <c r="AX29">
-        <f t="shared" ref="AX29:BL29" si="59">AX25-AX27</f>
+        <f t="shared" ref="AX29:BA29" si="59">AX25-AX27</f>
         <v>10</v>
       </c>
       <c r="AY29">
@@ -1921,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="BC29">
-        <f t="shared" ref="BC29:BM29" si="60">BC25-BC27</f>
+        <f t="shared" ref="BC29" si="60">BC25-BC27</f>
         <v>-2</v>
       </c>
       <c r="BD29">
@@ -1929,7 +2025,7 @@
         <v>-17</v>
       </c>
       <c r="BE29">
-        <f t="shared" ref="BE29:BM29" si="61">BE25-BE27</f>
+        <f t="shared" ref="BE29:BJ29" si="61">BE25-BE27</f>
         <v>24</v>
       </c>
       <c r="BF29">
@@ -2108,6 +2204,340 @@
       <c r="BJ32" t="str">
         <f t="shared" si="77"/>
         <v>G</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73DFA73-5C41-434E-BD93-E1A2FEFF05CA}">
+  <dimension ref="B1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <f>LEN(C2)</f>
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <f>LEN(F2)</f>
+        <v>112</v>
+      </c>
+      <c r="J2">
+        <f>LEN(I2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <f>LEN(C3)</f>
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" si="0">LEN(F3)</f>
+        <v>112</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J15" si="1">LEN(I3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="F4" s="2"/>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D15" si="2">LEN(C5)</f>
+        <v>14</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>